<commit_message>
Got the form that I was looking for
</commit_message>
<xml_diff>
--- a/CH-040 Cross Selling.xlsx
+++ b/CH-040 Cross Selling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD0F802-875D-4DC4-BB23-804E66D6DE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EFE746-4D02-4592-AB06-26FE6D0CBFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$H$27:$L$37</definedName>
+    <definedName name="_nResult">Sheet1!$L$3:$L$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="34">
   <si>
     <t>Question</t>
   </si>
@@ -157,6 +158,12 @@
   </si>
   <si>
     <t>Complement</t>
+  </si>
+  <si>
+    <t>Factor 1</t>
+  </si>
+  <si>
+    <t>Factor 2</t>
   </si>
 </sst>
 </file>
@@ -166,7 +173,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dddd"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,8 +207,23 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Mono"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,14 +284,8 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -552,11 +568,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -659,6 +702,21 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="10" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -680,30 +738,34 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="10" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1257,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R57"/>
+  <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1276,23 +1338,26 @@
     <col min="10" max="10" width="11.296875" customWidth="1"/>
     <col min="11" max="11" width="12.59765625" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.69921875" customWidth="1"/>
+    <col min="15" max="16" width="0" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="46"/>
-      <c r="H1" s="49" t="s">
+      <c r="B1" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="51"/>
+      <c r="H1" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="48"/>
+      <c r="K1" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="53"/>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
@@ -1311,7 +1376,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="H2" s="50"/>
+      <c r="H2" s="55"/>
       <c r="I2" s="3"/>
       <c r="K2" s="7" t="s">
         <v>29</v>
@@ -2273,12 +2338,12 @@
       <c r="K40"/>
     </row>
     <row r="41" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="I41" s="54" t="s">
+      <c r="I41" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="J41" s="54"/>
-      <c r="K41" s="55"/>
-      <c r="L41" s="54"/>
+      <c r="J41" s="47"/>
+      <c r="K41" s="48"/>
+      <c r="L41" s="47"/>
     </row>
     <row r="42" spans="3:13" x14ac:dyDescent="0.25">
       <c r="H42" t="s">
@@ -2298,11 +2363,10 @@
       </c>
     </row>
     <row r="43" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H43" s="51" t="s">
+      <c r="H43" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="I43" s="56"/>
-      <c r="J43" s="56" cm="1">
+      <c r="J43" cm="1">
         <f t="array" ref="J43">SUM(($I$28:$I$37=1)*(J28:J37))</f>
         <v>4</v>
       </c>
@@ -2320,14 +2384,13 @@
       </c>
     </row>
     <row r="44" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H44" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="I44" s="56" cm="1">
+      <c r="H44" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="I44" cm="1">
         <f t="array" ref="I44">SUM(($J$28:$J$37=1)*(I28:I37))</f>
         <v>4</v>
       </c>
-      <c r="J44" s="56"/>
       <c r="K44" cm="1">
         <f t="array" ref="K44">SUM(($J$28:$J$37=1)*(K28:K37))</f>
         <v>5</v>
@@ -2342,7 +2405,7 @@
       </c>
     </row>
     <row r="45" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H45" s="52" t="s">
+      <c r="H45" s="45" t="s">
         <v>24</v>
       </c>
       <c r="I45" s="6" cm="1">
@@ -2367,7 +2430,7 @@
       </c>
     </row>
     <row r="46" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H46" s="52" t="s">
+      <c r="H46" s="45" t="s">
         <v>26</v>
       </c>
       <c r="K46" cm="1">
@@ -2384,7 +2447,7 @@
       </c>
     </row>
     <row r="47" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H47" s="53" t="s">
+      <c r="H47" s="46" t="s">
         <v>27</v>
       </c>
       <c r="J47" cm="1">
@@ -2401,138 +2464,327 @@
         <v>B</v>
       </c>
     </row>
-    <row r="51" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="I51" s="54" t="s">
+    <row r="50" spans="14:23" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O50" t="s">
+        <v>32</v>
+      </c>
+      <c r="P50" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q50" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="R50" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="S50" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="T50" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="U50" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="J51" s="54"/>
-      <c r="K51" s="55"/>
-      <c r="L51" s="54"/>
-    </row>
-    <row r="52" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H52" t="s">
-        <v>30</v>
-      </c>
-      <c r="I52" s="58" t="s">
+    </row>
+    <row r="51" spans="14:23" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="N51" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="J52" s="58" t="s">
-        <v>3</v>
-      </c>
-      <c r="K52" s="57" t="s">
+      <c r="O51" s="56" t="str" cm="1">
+        <f t="array" ref="O51">_xlfn.TEXTSPLIT(N51,",")</f>
+        <v>A</v>
+      </c>
+      <c r="P51" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q51" s="62" t="str" cm="1">
+        <f t="array" aca="1" ref="Q51" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P51,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O51,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(Q$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(Q$50,$N51)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
+        <v/>
+      </c>
+      <c r="R51" s="62" cm="1">
+        <f t="array" aca="1" ref="R51" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P51,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O51,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(R$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(R$50,$N51)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
         <v>4</v>
       </c>
-      <c r="L52" s="58" t="s">
+      <c r="S51" s="62" cm="1">
+        <f t="array" aca="1" ref="S51" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P51,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O51,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(S$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(S$50,$N51)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
+        <v>3</v>
+      </c>
+      <c r="T51" s="62" cm="1">
+        <f t="array" aca="1" ref="T51" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P51,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O51,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(T$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(T$50,$N51)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
+        <v>3</v>
+      </c>
+      <c r="U51" s="62" t="str">
+        <f ca="1">_xlfn.XLOOKUP(MAX(Q51:T51),Q51:T51,$Q$50:$T$50)</f>
+        <v>B</v>
+      </c>
+      <c r="W51" t="b" cm="1">
+        <f t="array" aca="1" ref="W51:W55" ca="1">_nResult=U51:U55</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="14:23" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="N52" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="O52" s="56" t="str" cm="1">
+        <f t="array" ref="O52">_xlfn.TEXTSPLIT(N52,",")</f>
+        <v>B</v>
+      </c>
+      <c r="P52" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q52" s="62" cm="1">
+        <f t="array" aca="1" ref="Q52" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P52,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O52,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(Q$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(Q$50,$N52)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
+        <v>4</v>
+      </c>
+      <c r="R52" s="62" t="str" cm="1">
+        <f t="array" aca="1" ref="R52" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P52,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O52,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(R$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(R$50,$N52)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
+        <v/>
+      </c>
+      <c r="S52" s="62" cm="1">
+        <f t="array" aca="1" ref="S52" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P52,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O52,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(S$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(S$50,$N52)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
+        <v>5</v>
+      </c>
+      <c r="T52" s="62" cm="1">
+        <f t="array" aca="1" ref="T52" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P52,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O52,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(T$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(T$50,$N52)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
+        <v>3</v>
+      </c>
+      <c r="U52" s="62" t="str">
+        <f t="shared" ref="U52:U55" ca="1" si="4">_xlfn.XLOOKUP(MAX(Q52:T52),Q52:T52,$I$42:$L$42)</f>
+        <v>C</v>
+      </c>
+      <c r="W52" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="14:23" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="N53" s="60" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="53" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H53" s="51" t="s">
+      <c r="O53" s="56" t="str" cm="1">
+        <f t="array" ref="O53">_xlfn.TEXTSPLIT(N53,",")</f>
+        <v>D</v>
+      </c>
+      <c r="P53" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q53" s="62" cm="1">
+        <f t="array" aca="1" ref="Q53" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P53,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O53,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(Q$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(Q$50,$N53)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
+        <v>3</v>
+      </c>
+      <c r="R53" s="62" cm="1">
+        <f t="array" aca="1" ref="R53" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P53,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O53,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(R$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(R$50,$N53)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
+        <v>3</v>
+      </c>
+      <c r="S53" s="62" cm="1">
+        <f t="array" aca="1" ref="S53" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P53,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O53,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(S$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(S$50,$N53)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
         <v>2</v>
       </c>
-      <c r="I53" s="56" t="str" cm="1">
-        <f t="array" aca="1" ref="I53" ca="1">IF($H53=I$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H53,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(I$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
+      <c r="T53" s="62" t="str" cm="1">
+        <f t="array" aca="1" ref="T53" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P53,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O53,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(T$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(T$50,$N53)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
         <v/>
       </c>
-      <c r="J53" s="56" cm="1">
-        <f t="array" aca="1" ref="J53" ca="1">IF($H53=J$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H53,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(J$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>4</v>
-      </c>
-      <c r="K53" s="56" cm="1">
-        <f t="array" aca="1" ref="K53" ca="1">IF($H53=K$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H53,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(K$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>3</v>
-      </c>
-      <c r="L53" s="56" cm="1">
-        <f t="array" aca="1" ref="L53" ca="1">IF($H53=L$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H53,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(L$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>3</v>
-      </c>
-      <c r="M53" t="str">
-        <f ca="1">_xlfn.XLOOKUP(MAX(I53:L53),I53:L53,$I$42:$L$42)</f>
+      <c r="U53" s="62" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>A</v>
+      </c>
+      <c r="W53" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="14:23" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="N54" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="O54" s="56" t="str" cm="1">
+        <f t="array" ref="O54:P54">_xlfn.TEXTSPLIT(N54,",")</f>
+        <v>A</v>
+      </c>
+      <c r="P54" s="56" t="str">
         <v>B</v>
       </c>
-    </row>
-    <row r="54" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H54" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="I54" s="56" cm="1">
-        <f t="array" aca="1" ref="I54" ca="1">IF($H54=I$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H54,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(I$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>4</v>
-      </c>
-      <c r="J54" s="56" t="str" cm="1">
-        <f t="array" aca="1" ref="J54" ca="1">IF($H54=J$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H54,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(J$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
+      <c r="Q54" s="62" t="str" cm="1">
+        <f t="array" aca="1" ref="Q54" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P54,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O54,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(Q$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(Q$50,$N54)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
         <v/>
       </c>
-      <c r="K54" s="56" cm="1">
-        <f t="array" aca="1" ref="K54" ca="1">IF($H54=K$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H54,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(K$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>5</v>
-      </c>
-      <c r="L54" s="56" cm="1">
-        <f t="array" aca="1" ref="L54" ca="1">IF($H54=L$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H54,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(L$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H55" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="I55" s="56" cm="1">
-        <f t="array" aca="1" ref="I55" ca="1">IF($H55=I$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H55,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(I$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>3</v>
-      </c>
-      <c r="J55" s="56" cm="1">
-        <f t="array" aca="1" ref="J55" ca="1">IF($H55=J$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H55,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(J$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>3</v>
-      </c>
-      <c r="K55" s="56" cm="1">
-        <f t="array" aca="1" ref="K55" ca="1">IF($H55=K$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H55,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(K$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>2</v>
-      </c>
-      <c r="L55" s="56" t="str" cm="1">
-        <f t="array" aca="1" ref="L55" ca="1">IF($H55=L$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H55,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(L$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
+      <c r="R54" s="62" t="str" cm="1">
+        <f t="array" aca="1" ref="R54" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P54,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O54,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(R$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(R$50,$N54)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
         <v/>
       </c>
-    </row>
-    <row r="56" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H56" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="I56" s="56" t="e" cm="1">
-        <f t="array" aca="1" ref="I56" ca="1">IF($H56=I$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H56,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(I$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J56" s="56" t="e" cm="1">
-        <f t="array" aca="1" ref="J56" ca="1">IF($H56=J$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H56,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(J$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K56" s="56" t="e" cm="1">
-        <f t="array" aca="1" ref="K56" ca="1">IF($H56=K$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H56,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(K$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L56" s="56" t="e" cm="1">
-        <f t="array" aca="1" ref="L56" ca="1">IF($H56=L$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H56,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(L$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="57" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H57" s="53" t="s">
+      <c r="S54" s="62" cm="1">
+        <f t="array" aca="1" ref="S54" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P54,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O54,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(S$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(S$50,$N54)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
+        <v>3</v>
+      </c>
+      <c r="T54" s="62" cm="1">
+        <f t="array" aca="1" ref="T54" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P54,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O54,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(T$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(T$50,$N54)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
+        <v>1</v>
+      </c>
+      <c r="U54" s="62" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>C</v>
+      </c>
+      <c r="W54" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="14:23" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="N55" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="I57" s="56" t="e" cm="1">
-        <f t="array" aca="1" ref="I57" ca="1">IF($H57=I$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H57,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(I$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J57" s="56" t="e" cm="1">
-        <f t="array" aca="1" ref="J57" ca="1">IF($H57=J$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H57,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(J$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K57" s="56" t="e" cm="1">
-        <f t="array" aca="1" ref="K57" ca="1">IF($H57=K$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H57,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(K$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L57" s="56" t="e" cm="1">
-        <f t="array" aca="1" ref="L57" ca="1">IF($H57=L$52,"",SUM(OFFSET($H$28,0,_xlfn.XMATCH($H57,_xlfn.ANCHORARRAY($I$27)),10,1)*OFFSET($H$28,0,_xlfn.XMATCH(L$52,_xlfn.ANCHORARRAY($I$27)),10,1)))</f>
-        <v>#N/A</v>
+      <c r="O55" s="56" t="str" cm="1">
+        <f t="array" ref="O55:P55">_xlfn.TEXTSPLIT(N55,",")</f>
+        <v>A</v>
+      </c>
+      <c r="P55" s="56" t="str">
+        <v>C</v>
+      </c>
+      <c r="Q55" s="63" t="str" cm="1">
+        <f t="array" aca="1" ref="Q55" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P55,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O55,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(Q$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(Q$50,$N55)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
+        <v/>
+      </c>
+      <c r="R55" s="63" cm="1">
+        <f t="array" aca="1" ref="R55" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P55,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O55,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(R$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(R$50,$N55)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
+        <v>3</v>
+      </c>
+      <c r="S55" s="63" t="str" cm="1">
+        <f t="array" aca="1" ref="S55" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P55,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O55,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(S$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(S$50,$N55)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
+        <v/>
+      </c>
+      <c r="T55" s="63" cm="1">
+        <f t="array" aca="1" ref="T55" ca="1">_xlfn.LET(
+_xlpm.first,OFFSET($H$28,0,_xlfn.XMATCH($P55,$I$42:$L$42),10,1),
+_xlpm.second,OFFSET($H$28,0,_xlfn.XMATCH($O55,$I$42:$L$42),10,1),
+_xlpm.flt,_xlpm.first*_xlpm.second,
+_xlpm.cmp, OFFSET($H$28,0,_xlfn.XMATCH(T$50,$I$42:$L$42),10,1),
+IF(ISNUMBER(FIND(T$50,$N55)),"",SUM(_xlpm.flt*_xlpm.cmp))
+)</f>
+        <v>1</v>
+      </c>
+      <c r="U55" s="63" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>B</v>
+      </c>
+      <c r="W55" t="b">
+        <f ca="1"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>